<commit_message>
Versión casi final 6°-1 y originales autor 4°-9
</commit_message>
<xml_diff>
--- a/seguimiento/Grado06.xlsx
+++ b/seguimiento/Grado06.xlsx
@@ -818,7 +818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -829,7 +829,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,9 +936,15 @@
       <c r="B6" s="4">
         <v>42086</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="5">
+        <v>42068</v>
+      </c>
+      <c r="D6" s="5">
+        <v>42068</v>
+      </c>
+      <c r="E6" s="5">
+        <v>42068</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>

</xml_diff>